<commit_message>
Worked on Duplicating the Different Hist Types
</commit_message>
<xml_diff>
--- a/HistogramDrill.xlsx
+++ b/HistogramDrill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EAEEE73-5D38-459D-A986-8872339E1F74}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783E8DB1-FCA6-46BA-9255-5B5D513FFAEE}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -19,11 +19,13 @@
   </sheets>
   <definedNames>
     <definedName name="_nData">Report!$C$16:$C$33</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Report!$C$16:$C$36</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Report!$C$16:$C$36</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -183,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;&lt;=&quot;0"/>
+    <numFmt numFmtId="164" formatCode="&quot;&lt;=&quot;0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -502,7 +504,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -515,23 +517,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -830,6 +828,1479 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chart Made</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Using Bar Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Report!$G$16:$G$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>&lt;=1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(1.0, 2.0]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(2.0, 3.0]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(3.0, 4.0]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&gt;4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Report!$H$16:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B265-4E35-B816-FDBCE0D48E92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="2"/>
+        <c:overlap val="-27"/>
+        <c:axId val="425185007"/>
+        <c:axId val="580152863"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="425185007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="580152863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="580152863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425185007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Chart Made Using Histogram Plot</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Consolas"/>
+            </a:rPr>
+            <a:t>Chart Made Using Histogram Plot</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{488F41AA-615E-442F-86DE-036ED8B6741E}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="1" overflow="4">
+              <cx:binCount val="5"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1046,6 +2517,164 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC88C461-57D4-6DC3-D587-2C137302BD59}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6629400" y="2695575"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>133709</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>91978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="A screenshot of a computer&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE5B015-F775-C1F7-9615-08E99A11E753}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11991975" y="2581275"/>
+          <a:ext cx="2572109" cy="3858163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>77152</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381952</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3C5CC01-E29D-8815-6E18-85EA62D8B6A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1096,6 +2725,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1177,7 +2810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1469,10 +3102,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:J39"/>
+  <dimension ref="B1:J36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1520,7 +3153,7 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1564,7 +3197,7 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1572,15 +3205,18 @@
       <c r="C16" s="9">
         <v>0.6</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <f>F13</f>
         <v>1</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17" cm="1">
+      <c r="G16" s="22">
+        <f>F16</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="15" cm="1">
         <f t="array" ref="H16:H20">FREQUENCY(C16:C36,F16:F19)</f>
         <v>5</v>
       </c>
@@ -1593,18 +3229,18 @@
       <c r="C17" s="9">
         <v>0.7</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <f>F16</f>
         <v>1</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="6">
         <v>2</v>
       </c>
-      <c r="G17" s="19" t="str">
+      <c r="G17" t="str">
         <f>_xlfn.CONCAT("(",TEXT(E17,"0.0"),", ",TEXT(F17,"0.0"),"]")</f>
         <v>(1.0, 2.0]</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="17">
         <v>7</v>
       </c>
     </row>
@@ -1612,18 +3248,18 @@
       <c r="C18" s="9">
         <v>0.8</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <f t="shared" ref="E18:E19" si="0">F17</f>
         <v>2</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="6">
         <v>3</v>
       </c>
-      <c r="G18" s="19" t="str">
+      <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="1">_xlfn.CONCAT("(",TEXT(E18,"0.0"),", ",TEXT(F18,"0.0"),"]")</f>
         <v>(2.0, 3.0]</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="17">
         <v>5</v>
       </c>
     </row>
@@ -1631,18 +3267,18 @@
       <c r="C19" s="9">
         <v>0.99990000000000001</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="6">
         <v>4</v>
       </c>
-      <c r="G19" s="19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="1"/>
         <v>(3.0, 4.0]</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1650,14 +3286,17 @@
       <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23">
+      <c r="G20" s="20" t="str">
+        <f>F20</f>
+        <v>&gt;4</v>
+      </c>
+      <c r="H20" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1721,29 +3360,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="9">
         <v>3.2</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="9">
         <v>4.2</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="9">
         <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I39">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1931,19 +3565,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1951,11 +3581,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1963,19 +3592,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1983,11 +3608,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1995,19 +3619,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -2015,11 +3635,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -2027,13 +3646,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I now have duplicated the FREQ plot
I am getting close to understanding how the hist plot works.
</commit_message>
<xml_diff>
--- a/HistogramDrill.xlsx
+++ b/HistogramDrill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783E8DB1-FCA6-46BA-9255-5B5D513FFAEE}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44AD2DF3-EC8B-4017-B934-65BAA70B2F68}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -19,13 +19,16 @@
   </sheets>
   <definedNames>
     <definedName name="_nData">Report!$C$16:$C$33</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Report!$C$16:$C$36</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Report!$C$58:$C$88</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Report!$C$16:$C$36</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Report!$C$58:$C$88</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Report!$C$58:$C$88</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Report!$C$58:$C$88</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>FROM:</t>
   </si>
@@ -179,13 +182,26 @@
   <si>
     <t>22-Jan-2024</t>
   </si>
+  <si>
+    <t>Let's look at my battery data example.</t>
+  </si>
+  <si>
+    <t>I don’t see a way to get percentages without some calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The hist plot does not support </t>
+  </si>
+  <si>
+    <t>using alternate cells for labels.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;&lt;=&quot;0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -484,7 +500,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -503,8 +519,9 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -530,8 +547,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="18" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
     <cellStyle name="Explanatory Text" xfId="17" builtinId="53"/>
@@ -548,6 +571,7 @@
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Output" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="18" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
@@ -1210,6 +1234,134 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>I Have Duplicated the Chart!</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Consolas"/>
+            </a:rPr>
+            <a:t>I Have Duplicated the Chart!</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{AA98DB18-1023-4D2C-80C1-0E66CD12B594}">
+          <cx:dataLabels/>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="18.75" overflow="19.25">
+              <cx:binCount val="4"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>I Have Duplicated the Chart!</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Consolas"/>
+            </a:rPr>
+            <a:t>I Have Duplicated the Chart!</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{AA98DB18-1023-4D2C-80C1-0E66CD12B594}">
+          <cx:dataLabels/>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="18.75" overflow="19.25">
+              <cx:binCount val="4"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1290,6 +1442,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -2297,6 +2529,1022 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2564,7 +3812,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6629400" y="2695575"/>
+              <a:off x="6631305" y="2695575"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2673,6 +3921,250 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>284867</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>55728</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="A graph of a number of bars&#10;&#10;Description automatically generated with medium confidence">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E5DA252-AF79-4050-57DB-4532AFBA4B27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11058525" y="7248525"/>
+          <a:ext cx="7327652" cy="3456153"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>300989</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Chart 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD9011B-BEE0-3FB3-23D5-2B50BC7D38B8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11582399" y="11003280"/>
+              <a:ext cx="6196965" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>93345</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Chart 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2CC3A0-5CD6-42AF-A15D-A255F46EA0A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11382375" y="14925675"/>
+              <a:ext cx="6189345" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>114656</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>76737</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="A screenshot of a computer&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4C9BC8E-8021-E7AD-AED8-8E0C72A99E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13211175" y="18011775"/>
+          <a:ext cx="2553056" cy="3848637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2810,7 +4302,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -3102,11 +4594,9 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:J36"/>
+  <dimension ref="B1:S94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3378,6 +4868,234 @@
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="9">
         <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="23"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>18.918333331666666</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>18.943333331666665</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>19.093333331666667</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>19.229166658333334</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>18.813333345</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>19.260833318333333</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>18.979999998333334</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>18.946666664999999</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>18.976666665</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>19.445833324999999</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>19.185833318333334</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>18.741666689999999</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>18.890833306666668</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>19.271666678333332</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>19.189999985</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>18.984999998333333</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>18.672499998333333</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>19.279166658333335</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>19.334999998333334</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>19.077500001666667</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>19.155833331666667</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>19.126666664999998</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>18.890833306666668</v>
+      </c>
+    </row>
+    <row r="81" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>18.658333356666667</v>
+      </c>
+    </row>
+    <row r="82" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>19.154166658333335</v>
+      </c>
+    </row>
+    <row r="83" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>19.164166665</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>18.929166665</v>
+      </c>
+    </row>
+    <row r="85" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>19.111666671666665</v>
+      </c>
+    </row>
+    <row r="86" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>18.705000011666666</v>
+      </c>
+      <c r="Q86" s="27">
+        <v>4</v>
+      </c>
+      <c r="R86" s="24">
+        <f>Q86/$Q$90</f>
+        <v>0.12903225806451613</v>
+      </c>
+      <c r="S86" t="str">
+        <f>Q86&amp;", "&amp;TEXT(R86,"0.0%")</f>
+        <v>4, 12.9%</v>
+      </c>
+    </row>
+    <row r="87" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>18.919999998333331</v>
+      </c>
+      <c r="Q87" s="27">
+        <v>11</v>
+      </c>
+      <c r="R87" s="24">
+        <f t="shared" ref="R87:R89" si="2">Q87/$Q$90</f>
+        <v>0.35483870967741937</v>
+      </c>
+      <c r="S87" t="str">
+        <f t="shared" ref="S87:S89" si="3">Q87&amp;", "&amp;TEXT(R87,"0.0%")</f>
+        <v>11, 35.5%</v>
+      </c>
+    </row>
+    <row r="88" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>19.274999991666668</v>
+      </c>
+      <c r="Q88" s="27">
+        <v>10</v>
+      </c>
+      <c r="R88" s="24">
+        <f t="shared" si="2"/>
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="S88" t="str">
+        <f t="shared" si="3"/>
+        <v>10, 32.3%</v>
+      </c>
+    </row>
+    <row r="89" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q89" s="28">
+        <v>6</v>
+      </c>
+      <c r="R89" s="26">
+        <f t="shared" si="2"/>
+        <v>0.19354838709677419</v>
+      </c>
+      <c r="S89" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>6, 19.4%</v>
+      </c>
+    </row>
+    <row r="90" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q90" s="27">
+        <f>SUM(Q86:Q89)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q94" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to figure out how to apply
More complex data
</commit_message>
<xml_diff>
--- a/HistogramDrill.xlsx
+++ b/HistogramDrill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA796E5F-9E93-46D6-ADB0-FAA4F798FF0C}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{68E416BE-3FCF-4DA2-B571-9D142B8F15A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9D70FE-7C0D-4D1F-845A-0AD06F2D688C}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,19 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$R$118:$R$149</definedName>
     <definedName name="_nData">Report!$C$16:$C$33</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Report!$C$16:$C$36</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Report!$C$58:$C$88</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Report!$AF$93</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Report!$C$58:$C$88</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Report!$T$104:$T$107</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Report!$C$58:$C$88</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Report!$T$104:$T$107</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Report!$R$119:$R$149</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Report!$C$16:$C$36</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Report!$C$58:$C$88</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Report!$T$104:$T$107</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Report!$C$58:$C$88</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Report!$R$119:$R$149</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="22" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>FROM:</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>I had to do one plot over the other. This is not a scalable approach.</t>
+  </si>
+  <si>
+    <t>List</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AD54DF8-BCA9-48B8-8B72-AB7389F2FCAA}" type="CELLRANGE">
+                    <a:fld id="{6C4ADE9E-41BF-4A42-8AFE-02E82B24B809}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1269,7 +1272,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{382A5D01-2704-48AC-A36F-030B80254111}" type="CELLRANGE">
+                    <a:fld id="{A0B7C779-8B16-42FE-9D1A-E7124C0404E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1303,7 +1306,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0131FC13-DA54-4F73-8FF8-3E731E2DB862}" type="CELLRANGE">
+                    <a:fld id="{8E0233AC-2B68-4C2B-AF3A-FF176FCE80F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1337,7 +1340,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0ADAC30-BB02-4D74-92A4-5B5B17FDD1E1}" type="CELLRANGE">
+                    <a:fld id="{1F57845F-459D-47A9-82B4-1663278C234C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1576,7 +1579,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1639,7 +1642,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1703,12 +1706,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1755,6 +1758,43 @@
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{F166D00A-B467-470E-81F0-E11191330920}">
+          <cx:dataLabels/>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="3.8099999999999996" overflow="3.8399999999999999">
+              <cx:binCount val="5"/>
+            </cx:binning>
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
@@ -1972,6 +2012,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -4511,6 +4591,514 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4818,9 +5406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>129899</xdr:colOff>
+      <xdr:colOff>133709</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>95788</xdr:rowOff>
+      <xdr:rowOff>91978</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4898,9 +5486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>288677</xdr:colOff>
+      <xdr:colOff>284867</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>59538</xdr:rowOff>
+      <xdr:rowOff>55728</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5098,9 +5686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>326111</xdr:colOff>
+      <xdr:colOff>322301</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>97692</xdr:rowOff>
+      <xdr:rowOff>93882</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5169,6 +5757,84 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365758</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>105727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>105727</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="Chart 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4243BEF-B0D3-3F9F-9435-48E1F7323748}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10528933" y="21032152"/>
+              <a:ext cx="6987541" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5219,10 +5885,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5304,7 +5966,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -5596,10 +6258,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:W112"/>
+  <dimension ref="B1:W149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y110" sqref="Y110"/>
+    <sheetView tabSelected="1" topLeftCell="I115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T120" sqref="T120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6200,7 +6862,168 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="118" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R118" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="119" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R119">
+        <v>3.8033100000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R120">
+        <v>3.8041499999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R121">
+        <v>3.8306200000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R122">
+        <v>3.8043</v>
+      </c>
+    </row>
+    <row r="123" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R123">
+        <v>3.80606</v>
+      </c>
+    </row>
+    <row r="124" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R124">
+        <v>3.8417599999999998</v>
+      </c>
+    </row>
+    <row r="125" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R125">
+        <v>3.8063600000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R126">
+        <v>3.8432900000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R127">
+        <v>3.8043800000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R128">
+        <v>3.8059099999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R129">
+        <v>3.80186</v>
+      </c>
+    </row>
+    <row r="130" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R130">
+        <v>3.8034599999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R131">
+        <v>3.8033100000000002</v>
+      </c>
+    </row>
+    <row r="132" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R132">
+        <v>3.8046799999999998</v>
+      </c>
+    </row>
+    <row r="133" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R133">
+        <v>3.8302399999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R134">
+        <v>3.8028499999999998</v>
+      </c>
+    </row>
+    <row r="135" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R135">
+        <v>3.8037700000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R136">
+        <v>3.80362</v>
+      </c>
+    </row>
+    <row r="137" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R137">
+        <v>3.8043800000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R138">
+        <v>3.8039200000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R139">
+        <v>3.8033100000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R140">
+        <v>3.8045300000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R141">
+        <v>3.8015599999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R142">
+        <v>3.8038500000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R143">
+        <v>3.8043800000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R144">
+        <v>3.8422999999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R145">
+        <v>3.8034599999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R146">
+        <v>3.8432900000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R147">
+        <v>3.8461099999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R148">
+        <v>3.8436699999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R149">
+        <v>3.80369</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="R118:R149" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6249,7 +7072,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-Jan-2024</v>
+        <v>24-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -6559,7 +7382,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-Jan-2024</v>
+        <v>24-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>